<commit_message>
Update Holiday Date && Update Ticket Price for Admin
</commit_message>
<xml_diff>
--- a/src/database/SystemSettings.xlsx
+++ b/src/database/SystemSettings.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnny/Desktop/SC2002_Assignment/src/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D59B28E-EBBD-EA46-8593-FA192A59A577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCE37D7-782B-1C46-9E1E-6AE48AC5A6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="1480" windowWidth="21260" windowHeight="13320" xr2:uid="{7EE58E70-27BD-D94D-8E58-E5F1FF074EE6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,18 +36,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>holidays</t>
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>1012022</t>
+  </si>
+  <si>
+    <t>1022022</t>
+  </si>
+  <si>
+    <t>2012022</t>
+  </si>
+  <si>
+    <t>2022022</t>
+  </si>
+  <si>
+    <t>9082022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -393,23 +421,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F670353-C318-F448-81C3-56E066257AEB}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.1640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="0">
+        <v>6012022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>